<commit_message>
Added part numbers for all parts
</commit_message>
<xml_diff>
--- a/Bill of Materials/core-bom.xlsx
+++ b/Bill of Materials/core-bom.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
     <sheet name="Quote sheet" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BOM!$A$1:$G$27</definedName>
     <definedName name="bom" localSheetId="0">BOM!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="114">
   <si>
     <t>Part</t>
   </si>
@@ -184,9 +184,6 @@
     <t>Dual NPN transistor</t>
   </si>
   <si>
-    <t>0402-RES</t>
-  </si>
-  <si>
     <t>R2</t>
   </si>
   <si>
@@ -292,9 +289,6 @@
     <t>R7, R11-13</t>
   </si>
   <si>
-    <t>BTN, RESET</t>
-  </si>
-  <si>
     <t>MIC5219 3.3V LDO</t>
   </si>
   <si>
@@ -329,22 +323,98 @@
   </si>
   <si>
     <t>Need</t>
+  </si>
+  <si>
+    <t>Spark Devices</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Store Name</t>
+  </si>
+  <si>
+    <t>商家名称</t>
+  </si>
+  <si>
+    <t>Store Location</t>
+  </si>
+  <si>
+    <t>地址</t>
+  </si>
+  <si>
+    <t>Store Contact Info</t>
+  </si>
+  <si>
+    <t>联系电话</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Total price</t>
+  </si>
+  <si>
+    <t>Spark Part #</t>
+  </si>
+  <si>
+    <t>数量</t>
+  </si>
+  <si>
+    <t>价格</t>
+  </si>
+  <si>
+    <t>总价</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>全价</t>
+  </si>
+  <si>
+    <t>B1, B2</t>
+  </si>
+  <si>
+    <t>English Description</t>
+  </si>
+  <si>
+    <t>STM32 Micro-controller</t>
+  </si>
+  <si>
+    <t>Looks like this: http://www.digikey.com/product-detail/en/KMR211GLFS/401-1426-1-ND/550461</t>
+  </si>
+  <si>
+    <t>Chang Feng Tai</t>
+  </si>
+  <si>
+    <t>SEG, Second Floor</t>
+  </si>
+  <si>
+    <t>QQ: 421017527</t>
+  </si>
+  <si>
+    <t>Spark Core v0.0.5</t>
+  </si>
+  <si>
+    <t>RB551V-30 (500mA)</t>
+  </si>
+  <si>
+    <t>MMZ1005Y121C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -367,6 +437,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -376,7 +470,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -384,64 +478,239 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="89">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -466,6 +735,26 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -490,6 +779,26 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -823,259 +1132,265 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.83203125" customWidth="1"/>
-    <col min="3" max="3" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1640625" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.83203125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="28.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.1640625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="8"/>
+    <col min="7" max="7" width="11.83203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" s="21" customFormat="1">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" customFormat="1" hidden="1">
       <c r="A2" t="s">
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="A3" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="8">
+        <v>2</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3">
+      <c r="B4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="8">
+        <v>3</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="8">
+        <v>7</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="8">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="G7" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F9" s="8">
+        <v>1</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" customFormat="1" hidden="1">
+      <c r="A10" t="s">
         <v>63</v>
       </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5">
-        <v>7</v>
-      </c>
-      <c r="G5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-      <c r="G7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" t="s">
         <v>64</v>
-      </c>
-      <c r="C10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" t="s">
-        <v>65</v>
       </c>
       <c r="F10">
         <v>2</v>
       </c>
       <c r="G10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" t="s">
+      <c r="A11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="8">
+        <v>1</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11">
+      <c r="D12" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="8">
         <v>1</v>
       </c>
-      <c r="G11" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="G12" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" customFormat="1" hidden="1">
+      <c r="A13" t="s">
         <v>69</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>70</v>
       </c>
       <c r="B13" t="s">
         <v>34</v>
@@ -1083,209 +1398,245 @@
       <c r="C13" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>71</v>
+      <c r="D13" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="F13">
         <v>2</v>
       </c>
+      <c r="G13" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" t="s">
+      <c r="A14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="8">
         <v>1</v>
       </c>
+      <c r="G14" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" t="s">
+      <c r="A15" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="8">
+        <v>4</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="8">
+        <v>1</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="8">
+        <v>1</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15">
+      <c r="D18" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="8">
+        <v>2</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="8">
+        <v>1</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16">
+      <c r="G20" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
-        <v>74</v>
-      </c>
-      <c r="B20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="G21" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" customFormat="1" hidden="1">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" t="s">
         <v>76</v>
       </c>
-      <c r="C21" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" t="s">
-        <v>78</v>
-      </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" t="s">
+      <c r="G22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="8">
+        <v>1</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C23" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23">
+      <c r="D24" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" t="s">
-        <v>80</v>
-      </c>
-      <c r="C24" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" t="s">
-        <v>82</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" customFormat="1" hidden="1">
       <c r="A25" t="s">
         <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D25" t="s">
         <v>14</v>
@@ -1293,10 +1644,13 @@
       <c r="F25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" customFormat="1" hidden="1">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
         <v>9</v>
@@ -1305,14 +1659,23 @@
         <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
+      <c r="G26" t="s">
+        <v>84</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G27"/>
+  <autoFilter ref="A1:G27">
+    <filterColumn colId="6">
+      <filters blank="1">
+        <filter val="Need"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -1325,15 +1688,684 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="8.83203125" style="8"/>
+    <col min="2" max="2" width="18" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.83203125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="2.83203125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="2.83203125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="2.83203125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" style="8" customWidth="1"/>
+    <col min="11" max="11" width="2.83203125" style="8" customWidth="1"/>
+    <col min="12" max="12" width="8.83203125" style="8"/>
+    <col min="13" max="13" width="2.83203125" style="8" customWidth="1"/>
+    <col min="14" max="14" width="8.83203125" style="8"/>
+    <col min="15" max="15" width="2.83203125" style="8" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.83203125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" s="2" customFormat="1" ht="13" thickBot="1">
+      <c r="B2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2" s="3">
+        <f ca="1">NOW()</f>
+        <v>41361.694965625</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14">
+      <c r="B3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+    </row>
+    <row r="4" spans="2:14" ht="16" thickBot="1">
+      <c r="B4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+    </row>
+    <row r="5" spans="2:14">
+      <c r="B5" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+    </row>
+    <row r="6" spans="2:14" ht="16" thickBot="1">
+      <c r="B6" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+    </row>
+    <row r="7" spans="2:14">
+      <c r="B7" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+    </row>
+    <row r="8" spans="2:14" ht="16" thickBot="1">
+      <c r="B8" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+    </row>
+    <row r="9" spans="2:14">
+      <c r="B9" s="2"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+    </row>
+    <row r="10" spans="2:14">
+      <c r="B10" s="2"/>
+      <c r="J10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" s="2" customFormat="1" ht="12">
+      <c r="B11" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14">
+      <c r="B12" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12" s="16">
+        <v>10</v>
+      </c>
+      <c r="K12" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="L12" s="16"/>
+      <c r="M12" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N12" s="16"/>
+    </row>
+    <row r="13" spans="2:14">
+      <c r="B13" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" s="16">
+        <v>1000</v>
+      </c>
+      <c r="K13" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="L13" s="16"/>
+      <c r="M13" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N13" s="16"/>
+    </row>
+    <row r="14" spans="2:14">
+      <c r="B14" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="J14" s="16">
+        <v>1000</v>
+      </c>
+      <c r="K14" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="L14" s="16"/>
+      <c r="M14" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N14" s="16"/>
+    </row>
+    <row r="15" spans="2:14">
+      <c r="B15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15" s="16">
+        <v>1000</v>
+      </c>
+      <c r="K15" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="L15" s="16"/>
+      <c r="M15" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N15" s="16"/>
+    </row>
+    <row r="16" spans="2:14">
+      <c r="B16" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="16">
+        <v>1000</v>
+      </c>
+      <c r="K16" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="L16" s="16"/>
+      <c r="M16" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N16" s="16"/>
+    </row>
+    <row r="17" spans="2:14">
+      <c r="B17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="16">
+        <v>10</v>
+      </c>
+      <c r="K17" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="L17" s="16"/>
+      <c r="M17" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N17" s="16"/>
+    </row>
+    <row r="18" spans="2:14">
+      <c r="B18" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="J18" s="16">
+        <v>10</v>
+      </c>
+      <c r="K18" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="L18" s="16"/>
+      <c r="M18" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N18" s="16"/>
+    </row>
+    <row r="19" spans="2:14">
+      <c r="B19" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="J19" s="16">
+        <v>10</v>
+      </c>
+      <c r="K19" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="L19" s="16"/>
+      <c r="M19" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N19" s="16"/>
+    </row>
+    <row r="20" spans="2:14">
+      <c r="B20" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" s="16">
+        <v>10</v>
+      </c>
+      <c r="K20" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="L20" s="16"/>
+      <c r="M20" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N20" s="16"/>
+    </row>
+    <row r="21" spans="2:14">
+      <c r="B21" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="J21" s="16">
+        <v>10</v>
+      </c>
+      <c r="K21" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="L21" s="16"/>
+      <c r="M21" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N21" s="16"/>
+    </row>
+    <row r="22" spans="2:14">
+      <c r="B22" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="J22" s="16">
+        <v>1000</v>
+      </c>
+      <c r="K22" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="L22" s="16"/>
+      <c r="M22" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N22" s="16"/>
+    </row>
+    <row r="23" spans="2:14">
+      <c r="B23" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="J23" s="16">
+        <v>1000</v>
+      </c>
+      <c r="K23" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="L23" s="16"/>
+      <c r="M23" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N23" s="16"/>
+    </row>
+    <row r="24" spans="2:14">
+      <c r="B24" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H24" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="J24" s="16">
+        <v>1000</v>
+      </c>
+      <c r="K24" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="L24" s="16"/>
+      <c r="M24" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N24" s="16"/>
+    </row>
+    <row r="25" spans="2:14">
+      <c r="B25" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="J25" s="16">
+        <v>1000</v>
+      </c>
+      <c r="K25" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="L25" s="16"/>
+      <c r="M25" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N25" s="16"/>
+    </row>
+    <row r="26" spans="2:14">
+      <c r="B26" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="J26" s="16">
+        <v>1000</v>
+      </c>
+      <c r="K26" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="L26" s="16"/>
+      <c r="M26" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N26" s="16"/>
+    </row>
+    <row r="27" spans="2:14">
+      <c r="B27" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="J27" s="16">
+        <v>1000</v>
+      </c>
+      <c r="K27" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="L27" s="16"/>
+      <c r="M27" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N27" s="16"/>
+    </row>
+    <row r="28" spans="2:14">
+      <c r="B28" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J28" s="16">
+        <v>10</v>
+      </c>
+      <c r="K28" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="L28" s="16"/>
+      <c r="M28" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N28" s="16"/>
+    </row>
+    <row r="29" spans="2:14">
+      <c r="B29" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J29" s="16">
+        <v>10</v>
+      </c>
+      <c r="K29" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="L29" s="16"/>
+      <c r="M29" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N29" s="16"/>
+    </row>
+    <row r="30" spans="2:14">
+      <c r="B30" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="J30" s="16">
+        <v>10</v>
+      </c>
+      <c r="K30" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="L30" s="16"/>
+      <c r="M30" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="N30" s="16"/>
+    </row>
+    <row r="31" spans="2:14">
+      <c r="B31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="12"/>
+    </row>
+    <row r="33" spans="12:14">
+      <c r="L33" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="N33" s="19"/>
+    </row>
+    <row r="34" spans="12:14">
+      <c r="L34" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="N34" s="20"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated TODO with Satish's feedback
</commit_message>
<xml_diff>
--- a/Bill of Materials/core-bom.xlsx
+++ b/Bill of Materials/core-bom.xlsx
@@ -1690,8 +1690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="N2" s="3">
         <f ca="1">NOW()</f>
-        <v>41361.694965625</v>
+        <v>41361.734317824077</v>
       </c>
     </row>
     <row r="3" spans="2:14">
@@ -1883,11 +1883,16 @@
       <c r="K12" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="L12" s="16"/>
+      <c r="L12" s="16">
+        <v>2.5</v>
+      </c>
       <c r="M12" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="N12" s="16"/>
+      <c r="N12" s="16">
+        <f>J12*L12</f>
+        <v>25</v>
+      </c>
     </row>
     <row r="13" spans="2:14">
       <c r="B13" s="8" t="s">
@@ -1903,16 +1908,21 @@
         <v>62</v>
       </c>
       <c r="J13" s="16">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="K13" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="L13" s="16"/>
+      <c r="L13" s="16">
+        <v>0.8</v>
+      </c>
       <c r="M13" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="N13" s="16"/>
+      <c r="N13" s="16">
+        <f t="shared" ref="N13:N30" si="0">J13*L13</f>
+        <v>80</v>
+      </c>
     </row>
     <row r="14" spans="2:14">
       <c r="B14" s="8" t="s">
@@ -1933,11 +1943,16 @@
       <c r="K14" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="L14" s="16"/>
+      <c r="L14" s="16">
+        <v>3.5000000000000003E-2</v>
+      </c>
       <c r="M14" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="N14" s="16"/>
+      <c r="N14" s="16">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="2:14">
       <c r="B15" s="8" t="s">
@@ -1958,11 +1973,16 @@
       <c r="K15" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="L15" s="16"/>
+      <c r="L15" s="16">
+        <v>3.5000000000000003E-2</v>
+      </c>
       <c r="M15" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="N15" s="16"/>
+      <c r="N15" s="16">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="16" spans="2:14">
       <c r="B16" s="8" t="s">
@@ -1983,11 +2003,16 @@
       <c r="K16" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="L16" s="16"/>
+      <c r="L16" s="16">
+        <v>3.5000000000000003E-2</v>
+      </c>
       <c r="M16" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="N16" s="16"/>
+      <c r="N16" s="16">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="17" spans="2:14">
       <c r="B17" s="8" t="s">
@@ -2008,11 +2033,16 @@
       <c r="K17" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="L17" s="16"/>
+      <c r="L17" s="16">
+        <v>2</v>
+      </c>
       <c r="M17" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="N17" s="16"/>
+      <c r="N17" s="16">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
     </row>
     <row r="18" spans="2:14">
       <c r="B18" s="8" t="s">
@@ -2033,11 +2063,16 @@
       <c r="K18" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="L18" s="16"/>
+      <c r="L18" s="16">
+        <v>1.5</v>
+      </c>
       <c r="M18" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="N18" s="16"/>
+      <c r="N18" s="16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="19" spans="2:14">
       <c r="B19" s="8" t="s">
@@ -2058,11 +2093,16 @@
       <c r="K19" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="L19" s="16"/>
+      <c r="L19" s="16">
+        <v>0.8</v>
+      </c>
       <c r="M19" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="N19" s="16"/>
+      <c r="N19" s="16">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="20" spans="2:14">
       <c r="B20" s="8" t="s">
@@ -2083,11 +2123,16 @@
       <c r="K20" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="L20" s="16"/>
+      <c r="L20" s="16">
+        <v>2.5</v>
+      </c>
       <c r="M20" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="N20" s="16"/>
+      <c r="N20" s="16">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="21" spans="2:14">
       <c r="B21" s="8" t="s">
@@ -2108,11 +2153,16 @@
       <c r="K21" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="L21" s="16"/>
+      <c r="L21" s="16">
+        <v>2</v>
+      </c>
       <c r="M21" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="N21" s="16"/>
+      <c r="N21" s="16">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
     </row>
     <row r="22" spans="2:14">
       <c r="B22" s="8" t="s">
@@ -2133,11 +2183,16 @@
       <c r="K22" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="L22" s="16"/>
+      <c r="L22" s="16">
+        <v>1.4999999999999999E-2</v>
+      </c>
       <c r="M22" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="N22" s="16"/>
+      <c r="N22" s="16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="23" spans="2:14">
       <c r="B23" s="8" t="s">
@@ -2158,11 +2213,16 @@
       <c r="K23" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="L23" s="16"/>
+      <c r="L23" s="16">
+        <v>1.4999999999999999E-2</v>
+      </c>
       <c r="M23" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="N23" s="16"/>
+      <c r="N23" s="16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="24" spans="2:14">
       <c r="B24" s="8" t="s">
@@ -2183,11 +2243,16 @@
       <c r="K24" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="L24" s="16"/>
+      <c r="L24" s="16">
+        <v>1.4999999999999999E-2</v>
+      </c>
       <c r="M24" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="N24" s="16"/>
+      <c r="N24" s="16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="25" spans="2:14">
       <c r="B25" s="8" t="s">
@@ -2208,11 +2273,16 @@
       <c r="K25" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="L25" s="16"/>
+      <c r="L25" s="16">
+        <v>1.4999999999999999E-2</v>
+      </c>
       <c r="M25" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="N25" s="16"/>
+      <c r="N25" s="16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="26" spans="2:14">
       <c r="B26" s="8" t="s">
@@ -2233,11 +2303,16 @@
       <c r="K26" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="L26" s="16"/>
+      <c r="L26" s="16">
+        <v>1.4999999999999999E-2</v>
+      </c>
       <c r="M26" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="N26" s="16"/>
+      <c r="N26" s="16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="27" spans="2:14">
       <c r="B27" s="8" t="s">
@@ -2258,11 +2333,16 @@
       <c r="K27" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="L27" s="16"/>
+      <c r="L27" s="16">
+        <v>1.4999999999999999E-2</v>
+      </c>
       <c r="M27" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="N27" s="16"/>
+      <c r="N27" s="16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="28" spans="2:14">
       <c r="B28" s="8" t="s">
@@ -2283,11 +2363,16 @@
       <c r="K28" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="L28" s="16"/>
+      <c r="L28" s="16">
+        <v>4.8</v>
+      </c>
       <c r="M28" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="N28" s="16"/>
+      <c r="N28" s="16">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
     </row>
     <row r="29" spans="2:14">
       <c r="B29" s="8" t="s">
@@ -2308,11 +2393,16 @@
       <c r="K29" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="L29" s="16"/>
+      <c r="L29" s="16">
+        <v>22</v>
+      </c>
       <c r="M29" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="N29" s="16"/>
+      <c r="N29" s="16">
+        <f t="shared" si="0"/>
+        <v>220</v>
+      </c>
     </row>
     <row r="30" spans="2:14">
       <c r="B30" s="8" t="s">
@@ -2333,11 +2423,16 @@
       <c r="K30" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="L30" s="16"/>
+      <c r="L30" s="16">
+        <v>7</v>
+      </c>
       <c r="M30" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="N30" s="16"/>
+      <c r="N30" s="16">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
     </row>
     <row r="31" spans="2:14">
       <c r="B31" s="4"/>
@@ -2355,7 +2450,10 @@
       <c r="L33" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="N33" s="19"/>
+      <c r="N33" s="19">
+        <f>SUM(N12:N30)</f>
+        <v>726</v>
+      </c>
     </row>
     <row r="34" spans="12:14">
       <c r="L34" s="8" t="s">

</xml_diff>